<commit_message>
Updated Sprint 16 backlog for Week 1
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint16Plan.xlsx
+++ b/doc/Planning/Sprint16Plan.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Comments" sheetId="2" r:id="rId2"/>
+    <sheet name="Week 1" sheetId="3" r:id="rId2"/>
+    <sheet name="Comments" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="71">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -169,9 +170,6 @@
     <t>ایجاد امکانات پایه مورد نیاز در سیستم امنیتی</t>
   </si>
   <si>
-    <t>ایجاد کنترل گرید با امکانات استاندارد مورد نیاز برای استفاده سراسری در برنامه</t>
-  </si>
-  <si>
     <t>امکان جابجا کردن ترتیب ستون ها در کنترل گرید</t>
   </si>
   <si>
@@ -218,6 +216,33 @@
   </si>
   <si>
     <t>مستندسازی روال های کار با فریم ورک</t>
+  </si>
+  <si>
+    <t>پیش بینی هفتگی</t>
+  </si>
+  <si>
+    <t>هفته های بعد</t>
+  </si>
+  <si>
+    <t>بررسی و آماده کردن کنترل های واسط کاربری</t>
+  </si>
+  <si>
+    <t>آماده کردن کنترل گرید برای نمایش اطلاعات چندسطحی</t>
+  </si>
+  <si>
+    <t>آماده کردن کنترل درختی (TreeView) برای کار با اطلاعات چندسطحی</t>
+  </si>
+  <si>
+    <t>آماده کردن کنترل خاص برای نمایش و انتخاب بردار حساب</t>
+  </si>
+  <si>
+    <t>هفته اول</t>
+  </si>
+  <si>
+    <t>رفع اشکالات موجود در فرم های حساب، سند و آرتیکل سند</t>
+  </si>
+  <si>
+    <t>پیش بینی هفته اول اسپرینت 16</t>
   </si>
 </sst>
 </file>
@@ -343,7 +368,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="31">
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -441,6 +466,179 @@
         <vertical style="thin">
           <color auto="1"/>
         </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
         <horizontal/>
       </border>
     </dxf>
@@ -599,8 +797,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G35" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="A2:G35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H39" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="A2:H39"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="هدف کاری" dataDxfId="25"/>
+    <tableColumn id="2" name="قابلیت" dataDxfId="24"/>
+    <tableColumn id="4" name="وضعیت پذیرش" dataDxfId="23"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="22"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="21"/>
+    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="20"/>
+    <tableColumn id="9" name="پیش بینی هفتگی" dataDxfId="19"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:G17" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A2:G17"/>
   <tableColumns count="7">
     <tableColumn id="1" name="هدف کاری" dataDxfId="12"/>
     <tableColumn id="2" name="قابلیت" dataDxfId="11"/>
@@ -614,7 +829,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A2:C9"/>
   <tableColumns count="3">
@@ -889,29 +1104,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.109375" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" customWidth="1"/>
+    <col min="2" max="2" width="57.77734375" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -931,10 +1147,13 @@
         <v>8</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
@@ -953,9 +1172,12 @@
       <c r="F3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
         <v>23</v>
@@ -972,9 +1194,12 @@
       <c r="F4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
         <v>24</v>
@@ -991,9 +1216,12 @@
       <c r="F5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="4" t="s">
         <v>25</v>
@@ -1010,9 +1238,12 @@
       <c r="F6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="4" t="s">
         <v>26</v>
@@ -1029,9 +1260,12 @@
       <c r="F7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="4" t="s">
         <v>27</v>
@@ -1048,9 +1282,12 @@
       <c r="F8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="4" t="s">
         <v>28</v>
@@ -1067,9 +1304,12 @@
       <c r="F9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="4" t="s">
         <v>29</v>
@@ -1086,9 +1326,12 @@
       <c r="F10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="4" t="s">
         <v>30</v>
@@ -1105,9 +1348,12 @@
       <c r="F11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
         <v>31</v>
@@ -1124,9 +1370,12 @@
       <c r="F12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="4" t="s">
         <v>32</v>
@@ -1143,9 +1392,12 @@
       <c r="F13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="4" t="s">
         <v>33</v>
@@ -1162,9 +1414,12 @@
       <c r="F14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
         <v>34</v>
@@ -1181,9 +1436,12 @@
       <c r="F15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
         <v>35</v>
@@ -1200,9 +1458,12 @@
       <c r="F16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="4" t="s">
         <v>36</v>
@@ -1219,9 +1480,12 @@
       <c r="F17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
         <v>38</v>
@@ -1238,9 +1502,12 @@
       <c r="F18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="s">
         <v>39</v>
@@ -1257,9 +1524,12 @@
       <c r="F19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="4" t="s">
         <v>40</v>
@@ -1276,77 +1546,87 @@
       <c r="F20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="5">
-        <v>1</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="F22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>17</v>
@@ -1360,12 +1640,17 @@
       <c r="F24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
+      <c r="G24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="B25" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>17</v>
@@ -1379,12 +1664,15 @@
       <c r="F25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>17</v>
@@ -1398,12 +1686,15 @@
       <c r="F26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>17</v>
@@ -1417,14 +1708,15 @@
       <c r="F27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>51</v>
-      </c>
+      <c r="G27" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
       <c r="B28" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>17</v>
@@ -1433,17 +1725,20 @@
         <v>1</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="4" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>17</v>
@@ -1452,17 +1747,20 @@
         <v>1</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="4" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>17</v>
@@ -1471,17 +1769,20 @@
         <v>1</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>17</v>
@@ -1490,21 +1791,22 @@
         <v>1</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>17</v>
@@ -1518,12 +1820,15 @@
       <c r="F32" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>17</v>
@@ -1532,19 +1837,20 @@
         <v>1</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="G33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
       <c r="B34" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>17</v>
@@ -1558,37 +1864,138 @@
       <c r="F34" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="5">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="5">
+        <v>1</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="5">
-        <v>1</v>
-      </c>
-      <c r="E35" s="5" t="s">
+      <c r="B38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="5">
+        <v>1</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="4"/>
+      <c r="F39" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D31 D32:D34">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D35 D36:D38">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C31 C32:C34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C35 C36:C38">
       <formula1>"پیشنهاد اولیه,درخواست جزئیات,پذیرش,عدم پذیرش,تعلیق"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F31 F32:F34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F36:F38 F3:F35">
       <formula1>"اسپرینت 16,اسپرینت های بعدی"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G39">
+      <formula1>"هفته اول,هفته دوم,هفته سوم,هفته های بعد"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1600,6 +2007,365 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.109375" customWidth="1"/>
+    <col min="2" max="2" width="57.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F16">
+      <formula1>"اسپرینت 16,اسپرینت های بعدی"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C16">
+      <formula1>"پیشنهاد اولیه,درخواست جزئیات,پذیرش,عدم پذیرش,تعلیق"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D16">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Removed previously generated code and related metadata (Build 267)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint16Plan.xlsx
+++ b/doc/Planning/Sprint16Plan.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="72">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>اعمال دسترسی های امنیتی کاربر جاری داخل برنامه</t>
-  </si>
-  <si>
-    <t>وضعیت پذیرش</t>
   </si>
   <si>
     <t>گزینه های موجود</t>
@@ -83,9 +80,6 @@
     <t>بابک اسلامیه</t>
   </si>
   <si>
-    <t>پیشنهاد اولیه</t>
-  </si>
-  <si>
     <t>سعید قاسمی</t>
   </si>
   <si>
@@ -243,6 +237,15 @@
   </si>
   <si>
     <t>پیش بینی هفته اول اسپرینت 16</t>
+  </si>
+  <si>
+    <t>وضعیت انجام</t>
+  </si>
+  <si>
+    <t>انجام نشده</t>
+  </si>
+  <si>
+    <t>در حال انجام</t>
   </si>
 </sst>
 </file>
@@ -339,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -364,12 +367,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="31">
     <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -519,23 +555,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -654,23 +673,6 @@
         <top/>
         <bottom/>
         <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
         <horizontal/>
       </border>
     </dxf>
@@ -802,40 +804,40 @@
   <tableColumns count="8">
     <tableColumn id="1" name="هدف کاری" dataDxfId="25"/>
     <tableColumn id="2" name="قابلیت" dataDxfId="24"/>
-    <tableColumn id="4" name="وضعیت پذیرش" dataDxfId="23"/>
-    <tableColumn id="5" name="اولویت" dataDxfId="22"/>
-    <tableColumn id="6" name="مسئول انجام" dataDxfId="21"/>
-    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="20"/>
-    <tableColumn id="9" name="پیش بینی هفتگی" dataDxfId="19"/>
-    <tableColumn id="7" name="توضیحات" dataDxfId="18"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="23"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="22"/>
+    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="21"/>
+    <tableColumn id="9" name="پیش بینی هفتگی" dataDxfId="20"/>
+    <tableColumn id="10" name="وضعیت انجام" dataDxfId="1"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:G17" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:G17" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A2:G17"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="هدف کاری" dataDxfId="12"/>
-    <tableColumn id="2" name="قابلیت" dataDxfId="11"/>
-    <tableColumn id="4" name="وضعیت پذیرش" dataDxfId="10"/>
-    <tableColumn id="5" name="اولویت" dataDxfId="9"/>
-    <tableColumn id="6" name="مسئول انجام" dataDxfId="8"/>
-    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="7"/>
-    <tableColumn id="7" name="توضیحات" dataDxfId="6"/>
+    <tableColumn id="1" name="هدف کاری" dataDxfId="13"/>
+    <tableColumn id="2" name="قابلیت" dataDxfId="12"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="11"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="10"/>
+    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="9"/>
+    <tableColumn id="3" name="وضعیت انجام" dataDxfId="0"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A2:C9"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="قابلیت" dataDxfId="2"/>
-    <tableColumn id="2" name="گزینه های موجود" dataDxfId="1"/>
-    <tableColumn id="3" name="توضیحات" dataDxfId="0"/>
+    <tableColumn id="1" name="قابلیت" dataDxfId="4"/>
+    <tableColumn id="2" name="گزینه های موجود" dataDxfId="3"/>
+    <tableColumn id="3" name="توضیحات" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1107,24 +1109,24 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.109375" customWidth="1"/>
     <col min="2" max="2" width="57.77734375" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1135,19 +1137,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>3</v>
@@ -1155,847 +1157,849 @@
     </row>
     <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="5">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="5">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="5">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="5">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="5">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="5">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="5">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1</v>
+        <v>47</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="5">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="5">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="5">
-        <v>1</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="G31" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="5">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="5">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="5">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="5">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="H35" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="5">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="C36" s="5">
+        <v>1</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="5">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="C37" s="5">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="5">
+        <v>1</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="5">
-        <v>1</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="G38" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="5">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="C39" s="5">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H39" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D35 D36:D38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C35 C36:C38">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C35 C36:C38">
-      <formula1>"پیشنهاد اولیه,درخواست جزئیات,پذیرش,عدم پذیرش,تعلیق"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F36:F38 F3:F35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E36:E38 E3:E35">
       <formula1>"اسپرینت 16,اسپرینت های بعدی"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F39">
+      <formula1>"هفته اول,هفته دوم,هفته سوم,هفته های بعد"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G39">
-      <formula1>"هفته اول,هفته دوم,هفته سوم,هفته های بعد"</formula1>
+      <formula1>"انجام نشده,در حال انجام,انجام شده,در حال تست,تکمیل شده"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2008,26 +2012,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.109375" customWidth="1"/>
     <col min="2" max="2" width="57.77734375" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2038,16 +2042,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>3</v>
@@ -2055,312 +2059,379 @@
     </row>
     <row r="3" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F33" s="10"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F39" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E16">
       <formula1>"اسپرینت 16,اسپرینت های بعدی"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C16">
-      <formula1>"پیشنهاد اولیه,درخواست جزئیات,پذیرش,عدم پذیرش,تعلیق"</formula1>
+      <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D16">
-      <formula1>"1,2,3,4,5"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F39">
+      <formula1>"انجام نشده,در حال انجام,انجام شده,در حال تست,تکمیل شده"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2382,7 +2453,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="9"/>
     </row>
@@ -2391,7 +2462,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -2402,10 +2473,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
@@ -2413,10 +2484,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Implemented standard API for detail account + Week 1 status update (Build 272)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint16Plan.xlsx
+++ b/doc/Planning/Sprint16Plan.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="73">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -245,7 +245,10 @@
     <t>انجام نشده</t>
   </si>
   <si>
-    <t>در حال انجام</t>
+    <t>تکمیل شده</t>
+  </si>
+  <si>
+    <t>انجام شده</t>
   </si>
 </sst>
 </file>
@@ -269,12 +272,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -342,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -370,12 +385,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="31">
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -406,22 +539,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -438,9 +556,11 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -453,6 +573,37 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color auto="1"/>
@@ -469,10 +620,16 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -485,7 +642,9 @@
         <vertical style="thin">
           <color auto="1"/>
         </vertical>
-        <horizontal/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -517,132 +676,6 @@
         <top/>
         <bottom/>
         <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="medium">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
         <horizontal/>
       </border>
     </dxf>
@@ -808,36 +841,36 @@
     <tableColumn id="6" name="مسئول انجام" dataDxfId="22"/>
     <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="21"/>
     <tableColumn id="9" name="پیش بینی هفتگی" dataDxfId="20"/>
-    <tableColumn id="10" name="وضعیت انجام" dataDxfId="1"/>
-    <tableColumn id="7" name="توضیحات" dataDxfId="19"/>
+    <tableColumn id="10" name="وضعیت انجام" dataDxfId="19"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:G17" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:G17" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A2:G17"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="هدف کاری" dataDxfId="13"/>
-    <tableColumn id="2" name="قابلیت" dataDxfId="12"/>
-    <tableColumn id="5" name="اولویت" dataDxfId="11"/>
-    <tableColumn id="6" name="مسئول انجام" dataDxfId="10"/>
-    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="9"/>
-    <tableColumn id="3" name="وضعیت انجام" dataDxfId="0"/>
-    <tableColumn id="7" name="توضیحات" dataDxfId="8"/>
+    <tableColumn id="1" name="هدف کاری" dataDxfId="12"/>
+    <tableColumn id="2" name="قابلیت" dataDxfId="11"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="10"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="9"/>
+    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="8"/>
+    <tableColumn id="3" name="وضعیت انجام" dataDxfId="7"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A2:C9"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="قابلیت" dataDxfId="4"/>
-    <tableColumn id="2" name="گزینه های موجود" dataDxfId="3"/>
-    <tableColumn id="3" name="توضیحات" dataDxfId="2"/>
+    <tableColumn id="1" name="قابلیت" dataDxfId="2"/>
+    <tableColumn id="2" name="گزینه های موجود" dataDxfId="1"/>
+    <tableColumn id="3" name="توضیحات" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2015,7 +2048,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2136,23 +2169,23 @@
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="4"/>
+      <c r="E7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
@@ -2271,44 +2304,44 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="13">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="5" t="s">
+      <c r="E14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="G14" s="4"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C15" s="13">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="E15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
@@ -2325,7 +2358,7 @@
         <v>18</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G16" s="4"/>
     </row>

</xml_diff>

<commit_message>
[Refactoring] : Globally renamed 'transaction' to 'voucher' (Build 273)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint16Plan.xlsx
+++ b/doc/Planning/Sprint16Plan.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="74">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>انجام شده</t>
+  </si>
+  <si>
+    <t>در حال انجام</t>
   </si>
 </sst>
 </file>
@@ -2048,7 +2051,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2169,23 +2172,23 @@
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="16">
-        <v>1</v>
-      </c>
-      <c r="D7" s="16" t="s">
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="16" t="s">
+      <c r="E7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
@@ -2344,23 +2347,23 @@
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="5">
-        <v>1</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="4"/>
+      <c r="E16" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">

</xml_diff>

<commit_message>
Completed validation logic for voucher and voucher line APIs (Build 275)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint16Plan.xlsx
+++ b/doc/Planning/Sprint16Plan.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="73">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -249,9 +249,6 @@
   </si>
   <si>
     <t>انجام شده</t>
-  </si>
-  <si>
-    <t>در حال انجام</t>
   </si>
 </sst>
 </file>
@@ -275,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,12 +282,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -395,15 +386,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2051,7 +2033,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2191,42 +2173,42 @@
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4" t="s">
+      <c r="E8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="4"/>
+      <c r="E9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
@@ -2347,23 +2329,23 @@
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="13">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" s="15"/>
+      <c r="E16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">

</xml_diff>

<commit_message>
Updated sprint backlog for week 2
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint16Plan.xlsx
+++ b/doc/Planning/Sprint16Plan.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Week 1" sheetId="3" r:id="rId2"/>
-    <sheet name="Comments" sheetId="2" r:id="rId3"/>
+    <sheet name="Week 2" sheetId="4" r:id="rId3"/>
+    <sheet name="Comments" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="77">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -249,6 +250,18 @@
   </si>
   <si>
     <t>انجام شده</t>
+  </si>
+  <si>
+    <t>در حال انجام</t>
+  </si>
+  <si>
+    <t>پیش بینی هفته دوم اسپرینت 16</t>
+  </si>
+  <si>
+    <t>هفته دوم</t>
+  </si>
+  <si>
+    <t>امکان مدیریت اطلاعات سرفصل های حسابداری با ساختار درختی</t>
   </si>
 </sst>
 </file>
@@ -392,7 +405,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="42">
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -477,6 +490,194 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -646,21 +847,6 @@
         <vertical style="thin">
           <color auto="1"/>
         </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
         <horizontal/>
       </border>
     </dxf>
@@ -817,25 +1003,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H39" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="A2:H39"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="هدف کاری" dataDxfId="25"/>
-    <tableColumn id="2" name="قابلیت" dataDxfId="24"/>
-    <tableColumn id="5" name="اولویت" dataDxfId="23"/>
-    <tableColumn id="6" name="مسئول انجام" dataDxfId="22"/>
-    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="21"/>
-    <tableColumn id="9" name="پیش بینی هفتگی" dataDxfId="20"/>
-    <tableColumn id="10" name="وضعیت انجام" dataDxfId="19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G40" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+  <autoFilter ref="A2:G40"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="هدف کاری" dataDxfId="36"/>
+    <tableColumn id="2" name="قابلیت" dataDxfId="35"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="34"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="33"/>
+    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="32"/>
+    <tableColumn id="9" name="پیش بینی هفتگی" dataDxfId="31"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="30"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:G17" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="A2:G17"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="هدف کاری" dataDxfId="24"/>
+    <tableColumn id="2" name="قابلیت" dataDxfId="23"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="22"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="21"/>
+    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="20"/>
+    <tableColumn id="3" name="وضعیت انجام" dataDxfId="19"/>
     <tableColumn id="7" name="توضیحات" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:G17" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="A2:G17"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table146" displayName="Table146" ref="A2:G19" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A2:G19"/>
   <tableColumns count="7">
     <tableColumn id="1" name="هدف کاری" dataDxfId="12"/>
     <tableColumn id="2" name="قابلیت" dataDxfId="11"/>
@@ -849,7 +1050,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A2:C9"/>
   <tableColumns count="3">
@@ -1124,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1138,16 +1339,15 @@
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.5546875" customWidth="1"/>
+    <col min="7" max="7" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1167,13 +1367,10 @@
         <v>60</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>35</v>
       </c>
@@ -1192,12 +1389,9 @@
       <c r="F3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
         <v>21</v>
@@ -1214,12 +1408,9 @@
       <c r="F4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
         <v>22</v>
@@ -1236,12 +1427,9 @@
       <c r="F5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="4" t="s">
         <v>23</v>
@@ -1258,12 +1446,9 @@
       <c r="F6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="4" t="s">
         <v>24</v>
@@ -1278,14 +1463,11 @@
         <v>18</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="4" t="s">
         <v>25</v>
@@ -1300,14 +1482,11 @@
         <v>18</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="4" t="s">
         <v>26</v>
@@ -1322,14 +1501,11 @@
         <v>18</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="4" t="s">
         <v>27</v>
@@ -1344,14 +1520,11 @@
         <v>18</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="4" t="s">
         <v>28</v>
@@ -1366,14 +1539,11 @@
         <v>18</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
         <v>29</v>
@@ -1388,14 +1558,11 @@
         <v>18</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="4" t="s">
         <v>30</v>
@@ -1410,14 +1577,11 @@
         <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="4" t="s">
         <v>31</v>
@@ -1432,17 +1596,14 @@
         <v>18</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -1454,17 +1615,14 @@
         <v>18</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -1476,17 +1634,14 @@
         <v>18</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -1498,61 +1653,52 @@
         <v>18</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -1566,23 +1712,18 @@
       <c r="F20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="4" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>18</v>
@@ -1590,87 +1731,75 @@
       <c r="F21" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="G21" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="5" t="s">
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C24" s="5">
-        <v>1</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C25" s="5">
         <v>1</v>
@@ -1682,17 +1811,16 @@
         <v>18</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="B26" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
@@ -1706,15 +1834,12 @@
       <c r="F26" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="5">
         <v>1</v>
@@ -1728,15 +1853,12 @@
       <c r="F27" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="5">
         <v>1</v>
@@ -1750,43 +1872,37 @@
       <c r="F28" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C29" s="5">
         <v>1</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>18</v>
@@ -1794,15 +1910,12 @@
       <c r="F30" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="5">
         <v>1</v>
@@ -1816,23 +1929,18 @@
       <c r="F31" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
       <c r="B32" s="4" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="C32" s="5">
         <v>1</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>18</v>
@@ -1840,15 +1948,14 @@
       <c r="F32" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="B33" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="5">
         <v>1</v>
@@ -1862,15 +1969,12 @@
       <c r="F33" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" s="5">
         <v>1</v>
@@ -1884,15 +1988,12 @@
       <c r="F34" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="5">
         <v>1</v>
@@ -1904,21 +2005,14 @@
         <v>18</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
-        <v>54</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
       <c r="B36" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C36" s="5">
         <v>1</v>
@@ -1930,23 +2024,24 @@
         <v>18</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="B37" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" s="5">
         <v>1</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>18</v>
@@ -1954,23 +2049,18 @@
       <c r="F37" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G37" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
       <c r="B38" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" s="5">
         <v>1</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>18</v>
@@ -1978,46 +2068,58 @@
       <c r="F38" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G38" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="B39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="5">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="5">
-        <v>1</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="C40" s="5">
+        <v>1</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H39" s="4"/>
+      <c r="E40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G40" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C35 C36:C38">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C36 C37:C39">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E36:E38 E3:E35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E37:E39 E3:E36">
       <formula1>"اسپرینت 16,اسپرینت های بعدی"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F40">
       <formula1>"هفته اول,هفته دوم,هفته سوم,هفته های بعد"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G39">
-      <formula1>"انجام نشده,در حال انجام,انجام شده,در حال تست,تکمیل شده"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2032,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2076,82 +2178,82 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="4"/>
+      <c r="E3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="4"/>
+      <c r="E4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="4"/>
+      <c r="E5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="4"/>
+      <c r="E6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
@@ -2225,68 +2327,68 @@
         <v>18</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="4"/>
+      <c r="E11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="13">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" s="4"/>
+      <c r="E12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="4"/>
+      <c r="E13" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
@@ -2456,6 +2558,476 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.109375" customWidth="1"/>
+    <col min="2" max="2" width="58.44140625" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F33" s="10"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F41" s="10"/>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F19:F41">
+      <formula1>"انجام نشده,در حال انجام,انجام شده,در حال تست,تکمیل شده"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C18">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E18">
+      <formula1>"اسپرینت 16,اسپرینت های بعدی"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F18">
+      <formula1>"انجام نشده,در حال انجام,انجام شده,در حال تست,تکمیل شده"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">

</xml_diff>

<commit_message>
Implemented standard API for project + Week 2 status update (Build 277)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint16Plan.xlsx
+++ b/doc/Planning/Sprint16Plan.xlsx
@@ -2561,7 +2561,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2777,42 +2777,42 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="13">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" s="4"/>
+      <c r="E12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="4"/>
+      <c r="E13" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>

</xml_diff>

<commit_message>
Added new framework tool -> ProjectCLI (Build 280)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint16Plan.xlsx
+++ b/doc/Planning/Sprint16Plan.xlsx
@@ -285,7 +285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +295,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -399,6 +405,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2560,8 +2575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2758,23 +2773,23 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="4"/>
+      <c r="E11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
@@ -2895,25 +2910,25 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="16">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="4" t="s">
+      <c r="E18" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="15" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated sprint backlog for week 3
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint16Plan.xlsx
+++ b/doc/Planning/Sprint16Plan.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Week 1" sheetId="3" r:id="rId2"/>
     <sheet name="Week 2" sheetId="4" r:id="rId3"/>
-    <sheet name="Comments" sheetId="2" r:id="rId4"/>
+    <sheet name="Week 3" sheetId="5" r:id="rId4"/>
+    <sheet name="Comments" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="88">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -216,9 +217,6 @@
     <t>پیش بینی هفتگی</t>
   </si>
   <si>
-    <t>هفته های بعد</t>
-  </si>
-  <si>
     <t>بررسی و آماده کردن کنترل های واسط کاربری</t>
   </si>
   <si>
@@ -262,6 +260,42 @@
   </si>
   <si>
     <t>امکان مدیریت اطلاعات سرفصل های حسابداری با ساختار درختی</t>
+  </si>
+  <si>
+    <t>پشتیبانی از واسط کاربری چندزبانه</t>
+  </si>
+  <si>
+    <t>آماده کردن متن های چندزبانه برای نام فیلدها در فایل های resx</t>
+  </si>
+  <si>
+    <t>هفته سوم</t>
+  </si>
+  <si>
+    <t>پیش بینی هفته سوم اسپرینت 16</t>
+  </si>
+  <si>
+    <t>این بخش برای یکسان سازی متن پیغام های اعتبارسنجی بین برنامه و سرویس مورد استفاده ابزار جدید قرار خواهد گرفت.</t>
+  </si>
+  <si>
+    <t>اعمال دسترسی های امنیتی در فرم های لیست و ویرایش سرفصل های حسابداری</t>
+  </si>
+  <si>
+    <t>اعمال دسترسی های امنیتی در فرم های لیست و ویرایش تفصیلی های شناور</t>
+  </si>
+  <si>
+    <t>اعمال دسترسی های امنیتی در فرم های لیست و ویرایش مراکز هزینه</t>
+  </si>
+  <si>
+    <t>اعمال دسترسی های امنیتی در فرم های لیست و ویرایش پروژه ها</t>
+  </si>
+  <si>
+    <t>اعمال دسترسی های امنیتی در فرم های لیست و ویرایش اسناد مالی</t>
+  </si>
+  <si>
+    <t>اعمال دسترسی های امنیتی در فرم های لیست و ویرایش کاربران</t>
+  </si>
+  <si>
+    <t>اعمال دسترسی های امنیتی در فرم های لیست و ویرایش نقش ها</t>
   </si>
 </sst>
 </file>
@@ -370,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -416,11 +450,208 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="54">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1018,24 +1249,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G40" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
-  <autoFilter ref="A2:G40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G41" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49">
+  <autoFilter ref="A2:G41"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="هدف کاری" dataDxfId="48"/>
+    <tableColumn id="2" name="قابلیت" dataDxfId="47"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="46"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="45"/>
+    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="44"/>
+    <tableColumn id="9" name="پیش بینی هفتگی" dataDxfId="43"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:G17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+  <autoFilter ref="A2:G17"/>
   <tableColumns count="7">
     <tableColumn id="1" name="هدف کاری" dataDxfId="36"/>
     <tableColumn id="2" name="قابلیت" dataDxfId="35"/>
     <tableColumn id="5" name="اولویت" dataDxfId="34"/>
     <tableColumn id="6" name="مسئول انجام" dataDxfId="33"/>
     <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="32"/>
-    <tableColumn id="9" name="پیش بینی هفتگی" dataDxfId="31"/>
+    <tableColumn id="3" name="وضعیت انجام" dataDxfId="31"/>
     <tableColumn id="7" name="توضیحات" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:G17" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="A2:G17"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table146" displayName="Table146" ref="A2:G19" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="A2:G19"/>
   <tableColumns count="7">
     <tableColumn id="1" name="هدف کاری" dataDxfId="24"/>
     <tableColumn id="2" name="قابلیت" dataDxfId="23"/>
@@ -1049,29 +1296,29 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table146" displayName="Table146" ref="A2:G19" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="A2:G19"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1465" displayName="Table1465" ref="A2:G22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="A2:G22"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="هدف کاری" dataDxfId="12"/>
-    <tableColumn id="2" name="قابلیت" dataDxfId="11"/>
-    <tableColumn id="5" name="اولویت" dataDxfId="10"/>
-    <tableColumn id="6" name="مسئول انجام" dataDxfId="9"/>
-    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="8"/>
-    <tableColumn id="3" name="وضعیت انجام" dataDxfId="7"/>
-    <tableColumn id="7" name="توضیحات" dataDxfId="6"/>
+    <tableColumn id="1" name="هدف کاری" dataDxfId="6"/>
+    <tableColumn id="2" name="قابلیت" dataDxfId="5"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="4"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="3"/>
+    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="2"/>
+    <tableColumn id="3" name="وضعیت انجام" dataDxfId="1"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A2:C9"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="قابلیت" dataDxfId="2"/>
-    <tableColumn id="2" name="گزینه های موجود" dataDxfId="1"/>
-    <tableColumn id="3" name="توضیحات" dataDxfId="0"/>
+    <tableColumn id="1" name="قابلیت" dataDxfId="14"/>
+    <tableColumn id="2" name="گزینه های موجود" dataDxfId="13"/>
+    <tableColumn id="3" name="توضیحات" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1340,10 +1587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView rightToLeft="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1402,7 +1649,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -1421,7 +1668,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4" s="4"/>
     </row>
@@ -1440,7 +1687,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -1459,7 +1706,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -1478,7 +1725,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -1497,7 +1744,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -1516,7 +1763,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -1535,7 +1782,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -1554,7 +1801,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -1573,7 +1820,7 @@
         <v>18</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="4"/>
     </row>
@@ -1592,7 +1839,7 @@
         <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13" s="4"/>
     </row>
@@ -1611,14 +1858,14 @@
         <v>18</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -1630,7 +1877,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G15" s="4"/>
     </row>
@@ -1649,7 +1896,7 @@
         <v>18</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G16" s="4"/>
     </row>
@@ -1668,7 +1915,7 @@
         <v>18</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17" s="4"/>
     </row>
@@ -1687,7 +1934,7 @@
         <v>18</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -1706,7 +1953,7 @@
         <v>18</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G19" s="4"/>
     </row>
@@ -1725,7 +1972,7 @@
         <v>18</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G20" s="4"/>
     </row>
@@ -1744,7 +1991,7 @@
         <v>18</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>39</v>
@@ -1753,7 +2000,7 @@
     <row r="22" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
@@ -1765,7 +2012,7 @@
         <v>18</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G22" s="4"/>
     </row>
@@ -1786,7 +2033,7 @@
         <v>18</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G23" s="4"/>
     </row>
@@ -1805,7 +2052,7 @@
         <v>18</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>42</v>
@@ -1826,13 +2073,13 @@
         <v>18</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>44</v>
@@ -1847,7 +2094,7 @@
         <v>18</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="G26" s="4"/>
     </row>
@@ -1866,7 +2113,7 @@
         <v>18</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="G27" s="4"/>
     </row>
@@ -1885,7 +2132,7 @@
         <v>18</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="G28" s="4"/>
     </row>
@@ -1904,14 +2151,14 @@
         <v>18</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
@@ -1923,14 +2170,14 @@
         <v>18</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="5">
         <v>1</v>
@@ -1942,14 +2189,14 @@
         <v>18</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="5">
         <v>1</v>
@@ -1961,7 +2208,7 @@
         <v>18</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G32" s="4"/>
     </row>
@@ -1982,7 +2229,7 @@
         <v>18</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G33" s="4"/>
     </row>
@@ -2001,7 +2248,7 @@
         <v>18</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G34" s="4"/>
     </row>
@@ -2020,7 +2267,7 @@
         <v>18</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G35" s="4"/>
     </row>
@@ -2039,7 +2286,7 @@
         <v>18</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>53</v>
@@ -2062,7 +2309,7 @@
         <v>18</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="G37" s="4"/>
     </row>
@@ -2081,16 +2328,16 @@
         <v>18</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C39" s="5">
         <v>1</v>
@@ -2102,38 +2349,59 @@
         <v>18</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+    <row r="40" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="B40" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="5">
+        <v>1</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="5">
-        <v>1</v>
-      </c>
-      <c r="D40" s="5" t="s">
+      <c r="C41" s="5">
+        <v>1</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G40" s="4"/>
+      <c r="E41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G41" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C36 C37:C39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C36 C37:C40">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E37:E39 E3:E36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E37:E40 E3:E36">
       <formula1>"اسپرینت 16,اسپرینت های بعدی"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F41">
       <formula1>"هفته اول,هفته دوم,هفته سوم,هفته های بعد"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2150,7 +2418,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2166,7 +2434,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2186,7 +2454,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>3</v>
@@ -2209,7 +2477,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="12"/>
     </row>
@@ -2228,7 +2496,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="12"/>
     </row>
@@ -2247,7 +2515,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="12"/>
     </row>
@@ -2266,7 +2534,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" s="12"/>
     </row>
@@ -2285,7 +2553,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G7" s="12"/>
     </row>
@@ -2304,7 +2572,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" s="12"/>
     </row>
@@ -2323,35 +2591,35 @@
         <v>18</v>
       </c>
       <c r="F9" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="16">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="13">
         <v>1</v>
@@ -2363,14 +2631,14 @@
         <v>18</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="13">
         <v>1</v>
@@ -2382,14 +2650,14 @@
         <v>18</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="13">
         <v>1</v>
@@ -2401,7 +2669,7 @@
         <v>18</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G13" s="12"/>
     </row>
@@ -2422,7 +2690,7 @@
         <v>18</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G14" s="12"/>
     </row>
@@ -2441,7 +2709,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G15" s="12"/>
     </row>
@@ -2460,30 +2728,30 @@
         <v>18</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="19">
+        <v>1</v>
+      </c>
+      <c r="D17" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="4"/>
+      <c r="E17" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F18" s="10"/>
@@ -2575,8 +2843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2592,7 +2860,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2612,170 +2880,170 @@
         <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="4"/>
+      <c r="E3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="4"/>
+      <c r="E4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="4"/>
+      <c r="E5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="4"/>
+      <c r="E6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="4"/>
+      <c r="E7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="4"/>
+      <c r="E8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="4"/>
+      <c r="E9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="13">
+        <v>1</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="4"/>
+      <c r="E10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="13">
         <v>1</v>
@@ -2787,7 +3055,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="12"/>
     </row>
@@ -2806,7 +3074,7 @@
         <v>18</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="12"/>
     </row>
@@ -2825,28 +3093,28 @@
         <v>18</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="13">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="4"/>
+      <c r="E14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
@@ -2865,7 +3133,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15" s="4"/>
     </row>
@@ -2884,30 +3152,30 @@
         <v>18</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="13">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="4"/>
+      <c r="E17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
@@ -2926,32 +3194,32 @@
         <v>18</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G18" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="C19" s="16">
+        <v>1</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="4"/>
+      <c r="E19" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="15"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F20" s="10"/>
@@ -3043,6 +3311,524 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G44"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.109375" customWidth="1"/>
+    <col min="2" max="2" width="58.44140625" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="19">
+        <v>1</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="19">
+        <v>1</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="19">
+        <v>1</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="19">
+        <v>1</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="19">
+        <v>1</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="19">
+        <v>1</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="19">
+        <v>1</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="16">
+        <v>1</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:7" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F33" s="10"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F42" s="10"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F44" s="10"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E21:E22 E3:E19">
+      <formula1>"اسپرینت 16,اسپرینت های بعدی"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21:C22 C3:C19">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F44">
+      <formula1>"انجام نشده,در حال انجام,انجام شده,در حال تست,تکمیل شده"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">

</xml_diff>

<commit_message>
Fixed a typo in Persian resources + Status update
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint16Plan.xlsx
+++ b/doc/Planning/Sprint16Plan.xlsx
@@ -465,6 +465,89 @@
   </cellStyles>
   <dxfs count="54">
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -603,13 +686,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color auto="1"/>
@@ -635,6 +711,13 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -650,89 +733,6 @@
         <horizontal style="thin">
           <color auto="1"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="medium">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1297,28 +1297,28 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1465" displayName="Table1465" ref="A2:G22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1465" displayName="Table1465" ref="A2:G22" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A2:G22"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="هدف کاری" dataDxfId="6"/>
-    <tableColumn id="2" name="قابلیت" dataDxfId="5"/>
-    <tableColumn id="5" name="اولویت" dataDxfId="4"/>
-    <tableColumn id="6" name="مسئول انجام" dataDxfId="3"/>
-    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="2"/>
-    <tableColumn id="3" name="وضعیت انجام" dataDxfId="1"/>
-    <tableColumn id="7" name="توضیحات" dataDxfId="0"/>
+    <tableColumn id="1" name="هدف کاری" dataDxfId="12"/>
+    <tableColumn id="2" name="قابلیت" dataDxfId="11"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="10"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="9"/>
+    <tableColumn id="8" name="پیش بینی زمان انجام" dataDxfId="8"/>
+    <tableColumn id="3" name="وضعیت انجام" dataDxfId="7"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A2:C9"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="قابلیت" dataDxfId="14"/>
-    <tableColumn id="2" name="گزینه های موجود" dataDxfId="13"/>
-    <tableColumn id="3" name="توضیحات" dataDxfId="12"/>
+    <tableColumn id="1" name="قابلیت" dataDxfId="2"/>
+    <tableColumn id="2" name="گزینه های موجود" dataDxfId="1"/>
+    <tableColumn id="3" name="توضیحات" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2843,7 +2843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -3313,8 +3313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3496,25 +3496,25 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="C10" s="16">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
@@ -3711,25 +3711,25 @@
       <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="5">
-        <v>1</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="16">
+        <v>1</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" s="4" t="s">
+      <c r="E21" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="15" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>